<commit_message>
Updated ao_excel.py and ao_helper.py
Adding functions to ao_excel
Changed order in ao_helper
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,74 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\aoxlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16665" windowHeight="11370"/>
   </bookViews>
   <sheets>
-    <sheet name="Gold" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Fiber" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Gold" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Action</t>
   </si>
   <si>
     <t>Amount</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>Price/1</t>
   </si>
   <si>
-    <t>2017-05-06</t>
-  </si>
-  <si>
-    <t>Tier</t>
-  </si>
-  <si>
-    <t>Location</t>
+    <t>Price/total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt formatCode="General" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -83,32 +69,39 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+  <cellStyles count="1">
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,147 +389,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK13"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D14" activeCellId="0" pane="topLeft" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="11.85"/>
-    <col customWidth="1" max="1025" min="2" style="1" width="8.67"/>
+    <col min="1" max="1" width="11.875" style="2" customWidth="1"/>
+    <col min="2" max="4" width="8.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="1025" width="8.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="13.8" r="1" s="2" spans="1:3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row customHeight="1" ht="15" r="2" s="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="5" s="2" spans="1:3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="6" s="2" spans="1:3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="7" s="2" spans="1:3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C13" activeCellId="0" pane="topLeft" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0" outlineLevelRow="0"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="11.85"/>
-    <col customWidth="1" max="1025" min="2" style="1" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row customHeight="1" ht="12.8" r="1" s="2" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="5" s="2" spans="1:5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="6" s="2" spans="1:5">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="7" s="2" spans="1:5">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
-  <headerFooter differentFirst="0" differentOddEven="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to be committed: 	modified:   ao_excel.py 	modified:   ao_helper.py 	modified:   ao_main.py 	modified:   excel.xlsx
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\aoxlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16665" windowHeight="11370"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Gold" sheetId="1" r:id="rId1"/>
+    <sheet name="Gold" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Fibre" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -34,27 +30,61 @@
   </si>
   <si>
     <t>Price/total</t>
+  </si>
+  <si>
+    <t>Tier</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>2017-05-09</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>thetford</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt formatCode="General" numFmtId="164"/>
+    <numFmt formatCode="@" numFmtId="165"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -69,39 +99,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+  <cellXfs count="6">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -389,76 +421,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0"/>
   <cols>
-    <col min="1" max="1" width="11.875" style="2" customWidth="1"/>
-    <col min="2" max="4" width="8.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="1025" width="8.625" style="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="1" width="11.85"/>
+    <col customWidth="1" max="2" min="2" style="2" width="6.98"/>
+    <col customWidth="1" max="3" min="3" style="2" width="8.380000000000001"/>
+    <col customWidth="1" max="4" min="4" style="2" width="7.54"/>
+    <col customWidth="1" max="5" min="5" style="2" width="10.05"/>
+    <col customWidth="1" max="1025" min="6" style="2" width="8.630000000000001"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row customFormat="1" customHeight="1" ht="13.9" r="1" s="4" spans="1:5">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+    <row customHeight="1" ht="15" r="2" s="5" spans="1:5"/>
+    <row customHeight="1" ht="13.8" r="3" s="5" spans="1:5"/>
+    <row customHeight="1" ht="13.8" r="4" s="5" spans="1:5"/>
+    <row customHeight="1" ht="13.9" r="5" s="5" spans="1:5"/>
+    <row customHeight="1" ht="13.9" r="6" s="5" spans="1:5"/>
+    <row customHeight="1" ht="13.9" r="7" s="5" spans="1:5"/>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0" outlineLevelRow="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="2" width="11.85"/>
+    <col customWidth="1" max="4" min="2" style="2" width="8.67"/>
+    <col customWidth="1" max="5" min="5" style="2" width="10.05"/>
+    <col customWidth="1" max="1025" min="6" style="2" width="8.67"/>
+  </cols>
+  <sheetData>
+    <row customHeight="1" ht="15" r="1" s="5" spans="1:7">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row customHeight="1" ht="13.8" r="2" s="5" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="n">
+        <v>222</v>
+      </c>
+      <c r="D2" t="n">
+        <v>145.1891891891892</v>
+      </c>
+      <c r="E2" t="n">
+        <v>32232</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-    </row>
+    <row customHeight="1" ht="13.8" r="3" s="5" spans="1:7"/>
+    <row customHeight="1" ht="13.8" r="4" s="5" spans="1:7"/>
+    <row customHeight="1" ht="13.8" r="5" s="5" spans="1:7"/>
+    <row customHeight="1" ht="13.8" r="6" s="5" spans="1:7"/>
+    <row customHeight="1" ht="13.8" r="7" s="5" spans="1:7"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>